<commit_message>
fix: add recursion to Project Euler 5
</commit_message>
<xml_diff>
--- a/Project Euler 005.xlsx
+++ b/Project Euler 005.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noccis\Dropbox\1-projets\excel-problem-solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5632F2-C281-481E-B83E-9B81C585FE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1E825A-22C5-425B-9F69-4F9AE52BA19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D300F1E4-C82C-4AA2-99EB-33BA141A7AB9}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>Project Euler 5: Smallest Multiple</t>
   </si>
@@ -66,7 +66,16 @@
     <t>&lt;-- answer</t>
   </si>
   <si>
-    <t>with array formulas</t>
+    <t>1) Recursion</t>
+  </si>
+  <si>
+    <t>2) Tail-call recursion</t>
+  </si>
+  <si>
+    <t>3) With array formulas</t>
+  </si>
+  <si>
+    <t>4) Spreadsheets capabilities</t>
   </si>
 </sst>
 </file>
@@ -76,7 +85,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,6 +97,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="4"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -119,12 +144,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C4AECE-9570-4B27-85EC-0ACE3D221670}">
-  <dimension ref="B2:E6"/>
+  <dimension ref="B2:E40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -472,36 +501,225 @@
     <col min="6" max="6" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="2:5" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
+    <row r="4" spans="2:5" ht="16" x14ac:dyDescent="0.4">
+      <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B5" s="1">
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B6" s="1">
         <v>10</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D6" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B6" s="2" cm="1">
-        <f t="array" ref="B6">_xlfn.REDUCE(1,_xlfn.SEQUENCE(B5),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,LCM(_xlpm.a,_xlpm.v)))</f>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B7" s="2" cm="1">
+        <f t="array" ref="B7">_xlfn.LET(
+_xlpm.SUB, _xlfn.LAMBDA(_xlpm.ME,_xlpm.N,IF(_xlpm.N=1,1,LCM(_xlpm.N,_xlpm.ME(_xlpm.ME,_xlpm.N-1)))),
+_xlpm.SUB(_xlpm.SUB,B6))</f>
         <v>2520</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="4" cm="1">
-        <f t="array" ref="D6">_xlfn.REDUCE(1,_xlfn.SEQUENCE(D5),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,LCM(_xlpm.a,_xlpm.v)))</f>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3" cm="1">
+        <f t="array" ref="D7">_xlfn.LET(
+_xlpm.SUB, _xlfn.LAMBDA(_xlpm.ME,_xlpm.N,IF(_xlpm.N=1,1,LCM(_xlpm.N,_xlpm.ME(_xlpm.ME,_xlpm.N-1)))),
+_xlpm.SUB(_xlpm.SUB,D6))</f>
         <v>232792560</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="2:5" ht="16" x14ac:dyDescent="0.4">
+      <c r="B9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B11" s="1">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B12" s="2" cm="1">
+        <f t="array" ref="B12">_xlfn.LET(
+_xlpm.SUB, _xlfn.LAMBDA(_xlpm.ME,_xlpm.ACC,_xlpm.N, IF(_xlpm.N=1, _xlpm.ACC, _xlpm.ME(_xlpm.ME, LCM(_xlpm.ACC, _xlpm.N), _xlpm.N-1))),
+_xlpm.SUB(_xlpm.SUB,1,B11))</f>
+        <v>2520</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3" cm="1">
+        <f t="array" ref="D12">_xlfn.LET(
+_xlpm.SUB, _xlfn.LAMBDA(_xlpm.ME,_xlpm.ACC,_xlpm.N, IF(_xlpm.N=1, _xlpm.ACC, _xlpm.ME(_xlpm.ME, LCM(_xlpm.ACC, _xlpm.N), _xlpm.N-1))),
+_xlpm.SUB(_xlpm.SUB,1,D11))</f>
+        <v>232792560</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="16" x14ac:dyDescent="0.4">
+      <c r="B14" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B16" s="1">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" s="2" cm="1">
+        <f t="array" ref="B17">_xlfn.REDUCE(1,_xlfn.SEQUENCE(B16),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,LCM(_xlpm.a,_xlpm.v)))</f>
+        <v>2520</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="3" cm="1">
+        <f t="array" ref="D17">_xlfn.REDUCE(1,_xlfn.SEQUENCE(D16),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,LCM(_xlpm.a,_xlpm.v)))</f>
+        <v>232792560</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="16" x14ac:dyDescent="0.4">
+      <c r="B19" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3">
+        <f>LCM(B21:B40)</f>
+        <v>232792560</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B31">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B32">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B33">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B34">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B36">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B37">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B38">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B39">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B40">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: improve Project Euler 005
</commit_message>
<xml_diff>
--- a/Project Euler 005.xlsx
+++ b/Project Euler 005.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noccis\Dropbox\1-projets\excel-problem-solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B62831B-D2BB-4A73-A443-1EA201DCCD4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B73297B-9643-4ED1-8689-55792A5A041B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D300F1E4-C82C-4AA2-99EB-33BA141A7AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Project Euler 5: Smallest Multiple</t>
   </si>
@@ -107,13 +107,16 @@
     <t>2) One-liner based on tail-call recursion</t>
   </si>
   <si>
-    <t>3) One-liner based on array formulas</t>
-  </si>
-  <si>
-    <t>4) Use of spreadsheets capabilities</t>
-  </si>
-  <si>
     <t>(end)</t>
+  </si>
+  <si>
+    <t>4) One-liner based on array formulas</t>
+  </si>
+  <si>
+    <t>5) Use of spreadsheets capabilities</t>
+  </si>
+  <si>
+    <t>3) One-liner converting recursion into SEQUENCE+REDUCE</t>
   </si>
 </sst>
 </file>
@@ -556,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C4AECE-9570-4B27-85EC-0ACE3D221670}">
-  <dimension ref="B2:E46"/>
+  <dimension ref="B2:E51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -670,10 +673,22 @@
         <v>1</v>
       </c>
     </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="3"/>
+    </row>
     <row r="18" spans="2:5" ht="16" x14ac:dyDescent="0.4">
-      <c r="B18" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="B18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" s="1">
@@ -685,133 +700,165 @@
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="2" cm="1">
-        <f t="array" ref="B21">_xlfn.REDUCE(1, _xlfn.SEQUENCE(B20), _xlfn.LAMBDA(_xlpm.a,_xlpm.v, LCM(_xlpm.a,_xlpm.v)))</f>
+        <f t="array" ref="B21" xml:space="preserve"> _xlfn.REDUCE( 1, _xlfn.SEQUENCE(B20), _xlfn.LAMBDA(_xlpm.ACC,_xlpm.N, LCM(_xlpm.ACC,_xlpm.N)))</f>
         <v>2520</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="3" cm="1">
-        <f t="array" ref="D21">_xlfn.REDUCE(1, _xlfn.SEQUENCE(D20), _xlfn.LAMBDA(_xlpm.a,_xlpm.v, LCM(_xlpm.a,_xlpm.v)))</f>
+        <f t="array" ref="D21" xml:space="preserve"> _xlfn.REDUCE( 1, _xlfn.SEQUENCE(D20), _xlfn.LAMBDA(_xlpm.ACC,_xlpm.N, LCM(_xlpm.ACC,_xlpm.N)))</f>
         <v>232792560</v>
       </c>
       <c r="E21" t="s">
         <v>1</v>
       </c>
     </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="3"/>
+    </row>
     <row r="23" spans="2:5" ht="16" x14ac:dyDescent="0.4">
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B25">
+      <c r="B25" s="1">
+        <v>10</v>
+      </c>
+      <c r="D25" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B26" s="2" cm="1">
+        <f t="array" ref="B26">_xlfn.REDUCE(1, _xlfn.SEQUENCE(B25), _xlfn.LAMBDA(_xlpm.a,_xlpm.v, LCM(_xlpm.a,_xlpm.v)))</f>
+        <v>2520</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="3" cm="1">
+        <f t="array" ref="D26">_xlfn.REDUCE(1, _xlfn.SEQUENCE(D25), _xlfn.LAMBDA(_xlpm.a,_xlpm.v, LCM(_xlpm.a,_xlpm.v)))</f>
+        <v>232792560</v>
+      </c>
+      <c r="E26" t="s">
         <v>1</v>
       </c>
-      <c r="D25" s="3">
-        <f>LCM(B25:B44)</f>
-        <v>232792560</v>
-      </c>
-      <c r="E25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B28">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B29">
-        <v>5</v>
+    </row>
+    <row r="28" spans="2:5" ht="16" x14ac:dyDescent="0.4">
+      <c r="B28" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B30">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="D30" s="3">
+        <f>LCM(B30:B49)</f>
+        <v>232792560</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B31">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B32">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B35">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B36">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B37">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B38">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B39">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B40">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B41">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B42">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B43">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B44">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B46">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B47">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B48">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B49">
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B46" s="4" t="s">
-        <v>9</v>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B51" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>